<commit_message>
Remove start/end datetimes from IMC. Fix #561.
</commit_message>
<xml_diff>
--- a/docs/imc/imc-metadata.xlsx
+++ b/docs/imc/imc-metadata.xlsx
@@ -442,7 +442,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Time stamp indicating end of ablation for ROI</t>
+          <t>Image width value of the ROI acquisition</t>
         </r>
       </text>
     </comment>
@@ -455,7 +455,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Image width value of the ROI acquisition</t>
+          <t>Units of image width of the ROI acquisition</t>
         </r>
       </text>
     </comment>
@@ -468,7 +468,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Units of image width of the ROI acquisition</t>
+          <t>Image height value of the ROI acquisition</t>
         </r>
       </text>
     </comment>
@@ -481,7 +481,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Image height value of the ROI acquisition</t>
+          <t>Units of image height of the ROI acquisition</t>
         </r>
       </text>
     </comment>
@@ -494,7 +494,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Units of image height of the ROI acquisition</t>
+          <t>This refers to the data type, which is a "float" for the IMC counts.</t>
         </r>
       </text>
     </comment>
@@ -507,7 +507,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>This refers to the data type, which is a "float" for the IMC counts.</t>
+          <t>Type of signal measured per channel (usually dual counts)</t>
         </r>
       </text>
     </comment>
@@ -520,7 +520,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Type of signal measured per channel (usually dual counts)</t>
+          <t>Numerical data precision in bytes</t>
         </r>
       </text>
     </comment>
@@ -533,37 +533,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Time stamp indicating start of ablation for ROI</t>
+          <t>Relative path to file with ORCID IDs for contributors for this dataset.</t>
         </r>
       </text>
     </comment>
     <comment ref="AN1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Numerical data precision in bytes</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AO1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Relative path to file with ORCID IDs for contributors for this dataset.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AP1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -581,7 +555,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>version</t>
   </si>
@@ -697,9 +671,6 @@
     <t>dual_count_start</t>
   </si>
   <si>
-    <t>end_datetime</t>
-  </si>
-  <si>
     <t>max_x_width_value</t>
   </si>
   <si>
@@ -734,9 +705,6 @@
   </si>
   <si>
     <t>intensity value</t>
-  </si>
-  <si>
-    <t>start_datetime</t>
   </si>
   <si>
     <t>data_precision_bytes</t>
@@ -1094,7 +1062,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AP1"/>
+  <dimension ref="A1:AN1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1103,7 +1071,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:42">
+    <row r="1" spans="1:40">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1213,22 +1181,16 @@
         <v>42</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="AM1" s="1" t="s">
         <v>51</v>
       </c>
       <c r="AN1" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1281,27 +1243,27 @@
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AG2:AG1048576">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AF2:AF1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: um." sqref="AH2:AH1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: um." sqref="AG2:AG1048576">
       <formula1>'max_x_width_unit list'!$A$1:$A$1</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AI2:AI1048576">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AH2:AH1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: um." sqref="AJ2:AJ1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: um." sqref="AI2:AI1048576">
       <formula1>'max_y_height_unit list'!$A$1:$A$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: float / integer / string." sqref="AK2:AK1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: float / integer / string." sqref="AJ2:AJ1048576">
       <formula1>'segment_data_format list'!$A$1:$A$3</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: dual count / pulse count / intensity value." sqref="AL2:AL1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: dual count / pulse count / intensity value." sqref="AK2:AK1048576">
       <formula1>'signal_type list'!$A$1:$A$3</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AN2:AN1048576">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AL2:AL1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
@@ -1339,17 +1301,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1367,17 +1329,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
antibodies_path in IMC. Fix #551
</commit_message>
<xml_diff>
--- a/docs/imc/imc-metadata.xlsx
+++ b/docs/imc/imc-metadata.xlsx
@@ -533,11 +533,24 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>Relative path to file with antibody information for this dataset.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AN1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>Relative path to file with ORCID IDs for contributors for this dataset.</t>
         </r>
       </text>
     </comment>
-    <comment ref="AN1" authorId="0">
+    <comment ref="AO1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -555,7 +568,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
   <si>
     <t>version</t>
   </si>
@@ -708,6 +721,9 @@
   </si>
   <si>
     <t>data_precision_bytes</t>
+  </si>
+  <si>
+    <t>antibodies_path</t>
   </si>
   <si>
     <t>contributors_path</t>
@@ -1062,7 +1078,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AN1"/>
+  <dimension ref="A1:AO1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1071,7 +1087,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:40">
+    <row r="1" spans="1:41">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1191,6 +1207,9 @@
       </c>
       <c r="AN1" s="1" t="s">
         <v>52</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>